<commit_message>
updated several analysis scripts - added effect size calculations
</commit_message>
<xml_diff>
--- a/02_FDG_PET_data/Analysis/00_blood_glucose/stats_table_blood_glucose.xlsx
+++ b/02_FDG_PET_data/Analysis/00_blood_glucose/stats_table_blood_glucose.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -467,6 +467,11 @@
           <t>df</t>
         </is>
       </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>eta^2</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -504,6 +509,11 @@
           <t>(2, 10)</t>
         </is>
       </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>0.02</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -541,6 +551,11 @@
           <t>(2, 10)</t>
         </is>
       </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -578,6 +593,11 @@
           <t>(2, 10)</t>
         </is>
       </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>0.11</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -613,6 +633,11 @@
       <c r="G5" t="inlineStr">
         <is>
           <t>(2, 10)</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>0.11</t>
         </is>
       </c>
     </row>

</xml_diff>